<commit_message>
Atualização Documentação controle tabelas - NOVA e NIKE
</commit_message>
<xml_diff>
--- a/Documentação/Controle_Tabelas_e_Execucao/NIKE-Controle_tabelas.xlsx
+++ b/Documentação/Controle_Tabelas_e_Execucao/NIKE-Controle_tabelas.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="30" windowWidth="20115" windowHeight="8010" tabRatio="734"/>
+    <workbookView xWindow="240" yWindow="30" windowWidth="20115" windowHeight="8010" tabRatio="734" firstSheet="3" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Controladores Nike" sheetId="2" r:id="rId1"/>
@@ -16,13 +16,14 @@
     <sheet name="Estoque_Sige" sheetId="39" r:id="rId7"/>
     <sheet name="Relatorio Estoque" sheetId="42" r:id="rId8"/>
     <sheet name="Rentabilidade" sheetId="43" r:id="rId9"/>
+    <sheet name="Demais" sheetId="44" r:id="rId10"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1902" uniqueCount="561">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2017" uniqueCount="590">
   <si>
     <t>dtsx Principal</t>
   </si>
@@ -1705,6 +1706,93 @@
   </si>
   <si>
     <t>VW_NK_TRK_Status_Pedido</t>
+  </si>
+  <si>
+    <t>Nike_Carga</t>
+  </si>
+  <si>
+    <t>N:\Migracao\Nike_Carga\Nike_Carga\stg_nike.dtsx</t>
+  </si>
+  <si>
+    <t>(SC) STG  Nike</t>
+  </si>
+  <si>
+    <t>(DFT) Nike - Cliente Varejo</t>
+  </si>
+  <si>
+    <t>[nike].[stg_clientes_varejo]</t>
+  </si>
+  <si>
+    <t>(DFT) Nike - Estq Prod Entra Sai</t>
+  </si>
+  <si>
+    <t>[nike].[stg_estoque_prod_ent_sai]</t>
+  </si>
+  <si>
+    <t>(DFT) Nike - Estq Prod1 Entra Sai</t>
+  </si>
+  <si>
+    <t>[nike].[stg_estoque_prod1_ent_sai]</t>
+  </si>
+  <si>
+    <t>(DFT) Nike - Loja Entra Sai</t>
+  </si>
+  <si>
+    <t>[nike].[stg_loja_ent_sai]</t>
+  </si>
+  <si>
+    <t>(DFT) Nike - Loja Entra Sai Produto</t>
+  </si>
+  <si>
+    <t>[nike].[stg_loja_ent_sai_produto]</t>
+  </si>
+  <si>
+    <t>(DFT) Nike - Loja Imposto</t>
+  </si>
+  <si>
+    <t>[nike].[stg_loja_imposto]</t>
+  </si>
+  <si>
+    <t>(DFT) Nike - Loja NF</t>
+  </si>
+  <si>
+    <t>[nike].[stg_loja_nf]</t>
+  </si>
+  <si>
+    <t>(DFT) Nike - Loja NF Item</t>
+  </si>
+  <si>
+    <t>[nike].[stg_loja_nf_item]</t>
+  </si>
+  <si>
+    <t>(DFT) Nike - Loja Venda</t>
+  </si>
+  <si>
+    <t>[nike].[stg_loja_venda]</t>
+  </si>
+  <si>
+    <t>(DFT) Nike - Loja Venda Pagto</t>
+  </si>
+  <si>
+    <t>[nike].[stg_loja_venda_pagto]</t>
+  </si>
+  <si>
+    <t>(DFT) Nike - Loja Vda Pagto Parcelas</t>
+  </si>
+  <si>
+    <t>[nike].[stg_loja_venda_pagto_parcelas]</t>
+  </si>
+  <si>
+    <t>(DFT) Nike - Loja Vda Produto</t>
+  </si>
+  <si>
+    <t>[nike].[stg_loja_venda_produto]</t>
+  </si>
+  <si>
+    <t>(DFT) Nike - Loja Vda Troca</t>
+  </si>
+  <si>
+    <t>[nike].[stg_loja_venda_troca]</t>
   </si>
 </sst>
 </file>
@@ -2486,8 +2574,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25"/>
@@ -2797,6 +2885,734 @@
     <hyperlink ref="A5:A19" location="ssis_controlador_nike_SLA!A1" display="ssis_controlador_nike_SLA.dtsx"/>
     <hyperlink ref="A18" location="ssis_controlador_nike_SLA!A1" display="ssis_controlador_nike_SLA.dtsx"/>
   </hyperlinks>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:J39"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E18" sqref="E18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12"/>
+  <cols>
+    <col min="1" max="1" width="16.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="65" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="61.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="33.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.85546875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="40.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23.5703125" style="9" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" s="2" customFormat="1" ht="27.95" customHeight="1">
+      <c r="A1" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="22" t="s">
+        <v>156</v>
+      </c>
+      <c r="D1" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="E1" s="22" t="s">
+        <v>157</v>
+      </c>
+      <c r="F1" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="G1" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="H1" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="I1" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="J1" s="19" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" s="3" t="s">
+        <v>561</v>
+      </c>
+      <c r="B2" s="20"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="20" t="s">
+        <v>562</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>563</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>564</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>565</v>
+      </c>
+      <c r="J2" s="7"/>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" s="3" t="s">
+        <v>561</v>
+      </c>
+      <c r="B3" s="20"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="20" t="s">
+        <v>562</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>563</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>566</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>567</v>
+      </c>
+      <c r="J3" s="7"/>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" s="3" t="s">
+        <v>561</v>
+      </c>
+      <c r="B4" s="20"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="20" t="s">
+        <v>562</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>563</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>568</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>569</v>
+      </c>
+      <c r="J4" s="7"/>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" s="3" t="s">
+        <v>561</v>
+      </c>
+      <c r="B5" s="20"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="20" t="s">
+        <v>562</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>563</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>570</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>571</v>
+      </c>
+      <c r="J5" s="7"/>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" s="3" t="s">
+        <v>561</v>
+      </c>
+      <c r="B6" s="20"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="20" t="s">
+        <v>562</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>563</v>
+      </c>
+      <c r="G6" s="25" t="s">
+        <v>572</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>573</v>
+      </c>
+      <c r="J6" s="26"/>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" s="3" t="s">
+        <v>561</v>
+      </c>
+      <c r="B7" s="20"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="20" t="s">
+        <v>562</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>563</v>
+      </c>
+      <c r="G7" s="25" t="s">
+        <v>574</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>575</v>
+      </c>
+      <c r="J7" s="26"/>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" s="3" t="s">
+        <v>561</v>
+      </c>
+      <c r="B8" s="20"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="20" t="s">
+        <v>562</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>563</v>
+      </c>
+      <c r="G8" s="25" t="s">
+        <v>576</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>577</v>
+      </c>
+      <c r="J8" s="26"/>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9" s="3" t="s">
+        <v>561</v>
+      </c>
+      <c r="B9" s="20"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="20" t="s">
+        <v>562</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>563</v>
+      </c>
+      <c r="G9" s="25" t="s">
+        <v>578</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>579</v>
+      </c>
+      <c r="J9" s="26"/>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="A10" s="3" t="s">
+        <v>561</v>
+      </c>
+      <c r="B10" s="20"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="20" t="s">
+        <v>562</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>563</v>
+      </c>
+      <c r="G10" s="25" t="s">
+        <v>580</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="I10" s="4" t="s">
+        <v>581</v>
+      </c>
+      <c r="J10" s="26"/>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="A11" s="3" t="s">
+        <v>561</v>
+      </c>
+      <c r="B11" s="20"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="20" t="s">
+        <v>562</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>563</v>
+      </c>
+      <c r="G11" s="25" t="s">
+        <v>582</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="I11" s="4" t="s">
+        <v>583</v>
+      </c>
+      <c r="J11" s="26"/>
+    </row>
+    <row r="12" spans="1:10">
+      <c r="A12" s="3" t="s">
+        <v>561</v>
+      </c>
+      <c r="B12" s="20"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="20" t="s">
+        <v>562</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>563</v>
+      </c>
+      <c r="G12" s="25" t="s">
+        <v>584</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="I12" s="4" t="s">
+        <v>585</v>
+      </c>
+      <c r="J12" s="26"/>
+    </row>
+    <row r="13" spans="1:10">
+      <c r="A13" s="3" t="s">
+        <v>561</v>
+      </c>
+      <c r="B13" s="20"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="20" t="s">
+        <v>562</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>563</v>
+      </c>
+      <c r="G13" s="25" t="s">
+        <v>586</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="I13" s="4" t="s">
+        <v>587</v>
+      </c>
+      <c r="J13" s="26"/>
+    </row>
+    <row r="14" spans="1:10">
+      <c r="A14" s="3" t="s">
+        <v>561</v>
+      </c>
+      <c r="B14" s="20"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="20" t="s">
+        <v>562</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>563</v>
+      </c>
+      <c r="G14" s="25" t="s">
+        <v>588</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="I14" s="4" t="s">
+        <v>589</v>
+      </c>
+      <c r="J14" s="26"/>
+    </row>
+    <row r="15" spans="1:10">
+      <c r="A15" s="3" t="s">
+        <v>561</v>
+      </c>
+      <c r="B15" s="20"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="20"/>
+      <c r="F15" s="25"/>
+      <c r="G15" s="25"/>
+      <c r="H15" s="4"/>
+      <c r="I15" s="4"/>
+      <c r="J15" s="26"/>
+    </row>
+    <row r="16" spans="1:10">
+      <c r="A16" s="3" t="s">
+        <v>561</v>
+      </c>
+      <c r="B16" s="20"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="20"/>
+      <c r="F16" s="25"/>
+      <c r="G16" s="25"/>
+      <c r="H16" s="4"/>
+      <c r="I16" s="4"/>
+      <c r="J16" s="26"/>
+    </row>
+    <row r="17" spans="1:10">
+      <c r="A17" s="3" t="s">
+        <v>561</v>
+      </c>
+      <c r="B17" s="20"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="20"/>
+      <c r="F17" s="25"/>
+      <c r="G17" s="25"/>
+      <c r="H17" s="4"/>
+      <c r="I17" s="4"/>
+      <c r="J17" s="26"/>
+    </row>
+    <row r="18" spans="1:10">
+      <c r="A18" s="3" t="s">
+        <v>561</v>
+      </c>
+      <c r="B18" s="20"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="20"/>
+      <c r="F18" s="25"/>
+      <c r="G18" s="25"/>
+      <c r="H18" s="4"/>
+      <c r="I18" s="4"/>
+      <c r="J18" s="26"/>
+    </row>
+    <row r="19" spans="1:10">
+      <c r="A19" s="3" t="s">
+        <v>561</v>
+      </c>
+      <c r="B19" s="20"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="20"/>
+      <c r="F19" s="25"/>
+      <c r="G19" s="25"/>
+      <c r="H19" s="4"/>
+      <c r="I19" s="4"/>
+      <c r="J19" s="26"/>
+    </row>
+    <row r="20" spans="1:10">
+      <c r="A20" s="3" t="s">
+        <v>561</v>
+      </c>
+      <c r="B20" s="20"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="20"/>
+      <c r="F20" s="25"/>
+      <c r="G20" s="25"/>
+      <c r="H20" s="4"/>
+      <c r="I20" s="4"/>
+      <c r="J20" s="26"/>
+    </row>
+    <row r="21" spans="1:10">
+      <c r="A21" s="3" t="s">
+        <v>561</v>
+      </c>
+      <c r="B21" s="20"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="20"/>
+      <c r="F21" s="25"/>
+      <c r="G21" s="25"/>
+      <c r="H21" s="4"/>
+      <c r="I21" s="4"/>
+      <c r="J21" s="26"/>
+    </row>
+    <row r="22" spans="1:10">
+      <c r="A22" s="3" t="s">
+        <v>561</v>
+      </c>
+      <c r="B22" s="20"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="20"/>
+      <c r="F22" s="25"/>
+      <c r="G22" s="25"/>
+      <c r="H22" s="4"/>
+      <c r="I22" s="4"/>
+      <c r="J22" s="26"/>
+    </row>
+    <row r="23" spans="1:10">
+      <c r="A23" s="3" t="s">
+        <v>561</v>
+      </c>
+      <c r="B23" s="20"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="20"/>
+      <c r="F23" s="25"/>
+      <c r="G23" s="25"/>
+      <c r="H23" s="4"/>
+      <c r="I23" s="4"/>
+      <c r="J23" s="26"/>
+    </row>
+    <row r="24" spans="1:10">
+      <c r="A24" s="3" t="s">
+        <v>561</v>
+      </c>
+      <c r="B24" s="20"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="20"/>
+      <c r="F24" s="25"/>
+      <c r="G24" s="25"/>
+      <c r="H24" s="4"/>
+      <c r="I24" s="4"/>
+      <c r="J24" s="26"/>
+    </row>
+    <row r="25" spans="1:10">
+      <c r="A25" s="3" t="s">
+        <v>561</v>
+      </c>
+      <c r="B25" s="20"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="4"/>
+      <c r="E25" s="20"/>
+      <c r="F25" s="25"/>
+      <c r="G25" s="25"/>
+      <c r="H25" s="4"/>
+      <c r="I25" s="4"/>
+      <c r="J25" s="26"/>
+    </row>
+    <row r="26" spans="1:10">
+      <c r="A26" s="3" t="s">
+        <v>561</v>
+      </c>
+      <c r="B26" s="20"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="4"/>
+      <c r="E26" s="20"/>
+      <c r="F26" s="25"/>
+      <c r="G26" s="25"/>
+      <c r="H26" s="4"/>
+      <c r="I26" s="4"/>
+      <c r="J26" s="26"/>
+    </row>
+    <row r="27" spans="1:10">
+      <c r="A27" s="3" t="s">
+        <v>561</v>
+      </c>
+      <c r="B27" s="20"/>
+      <c r="C27" s="4"/>
+      <c r="D27" s="4"/>
+      <c r="E27" s="20"/>
+      <c r="F27" s="25"/>
+      <c r="G27" s="25"/>
+      <c r="H27" s="4"/>
+      <c r="I27" s="4"/>
+      <c r="J27" s="26"/>
+    </row>
+    <row r="28" spans="1:10">
+      <c r="A28" s="3" t="s">
+        <v>561</v>
+      </c>
+      <c r="B28" s="20"/>
+      <c r="C28" s="4"/>
+      <c r="D28" s="4"/>
+      <c r="E28" s="20"/>
+      <c r="F28" s="25"/>
+      <c r="G28" s="25"/>
+      <c r="H28" s="4"/>
+      <c r="I28" s="4"/>
+      <c r="J28" s="26"/>
+    </row>
+    <row r="29" spans="1:10">
+      <c r="A29" s="3" t="s">
+        <v>561</v>
+      </c>
+      <c r="B29" s="20"/>
+      <c r="C29" s="4"/>
+      <c r="D29" s="4"/>
+      <c r="E29" s="20"/>
+      <c r="F29" s="25"/>
+      <c r="G29" s="25"/>
+      <c r="H29" s="4"/>
+      <c r="I29" s="4"/>
+      <c r="J29" s="26"/>
+    </row>
+    <row r="30" spans="1:10">
+      <c r="A30" s="3" t="s">
+        <v>561</v>
+      </c>
+      <c r="B30" s="20"/>
+      <c r="C30" s="4"/>
+      <c r="D30" s="4"/>
+      <c r="E30" s="20"/>
+      <c r="F30" s="25"/>
+      <c r="G30" s="25"/>
+      <c r="H30" s="4"/>
+      <c r="I30" s="4"/>
+      <c r="J30" s="26"/>
+    </row>
+    <row r="31" spans="1:10">
+      <c r="A31" s="3" t="s">
+        <v>561</v>
+      </c>
+      <c r="B31" s="20"/>
+      <c r="C31" s="4"/>
+      <c r="D31" s="4"/>
+      <c r="E31" s="20"/>
+      <c r="F31" s="25"/>
+      <c r="G31" s="25"/>
+      <c r="H31" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="I31" s="4"/>
+      <c r="J31" s="26"/>
+    </row>
+    <row r="32" spans="1:10">
+      <c r="A32" s="3" t="s">
+        <v>561</v>
+      </c>
+      <c r="B32" s="20"/>
+      <c r="C32" s="4"/>
+      <c r="D32" s="4"/>
+      <c r="E32" s="20"/>
+      <c r="F32" s="25"/>
+      <c r="G32" s="25"/>
+      <c r="H32" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="I32" s="4"/>
+      <c r="J32" s="26"/>
+    </row>
+    <row r="33" spans="1:10">
+      <c r="A33" s="3" t="s">
+        <v>561</v>
+      </c>
+      <c r="B33" s="20"/>
+      <c r="C33" s="4"/>
+      <c r="D33" s="4"/>
+      <c r="E33" s="20"/>
+      <c r="F33" s="25"/>
+      <c r="G33" s="25"/>
+      <c r="H33" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="I33" s="4"/>
+      <c r="J33" s="26"/>
+    </row>
+    <row r="34" spans="1:10">
+      <c r="A34" s="3" t="s">
+        <v>561</v>
+      </c>
+      <c r="B34" s="20"/>
+      <c r="C34" s="4"/>
+      <c r="D34" s="4"/>
+      <c r="E34" s="20"/>
+      <c r="F34" s="25"/>
+      <c r="G34" s="25"/>
+      <c r="H34" s="4"/>
+      <c r="I34" s="4"/>
+      <c r="J34" s="26"/>
+    </row>
+    <row r="35" spans="1:10">
+      <c r="A35" s="3" t="s">
+        <v>561</v>
+      </c>
+      <c r="B35" s="20"/>
+      <c r="C35" s="4"/>
+      <c r="D35" s="4"/>
+      <c r="E35" s="20"/>
+      <c r="F35" s="25"/>
+      <c r="G35" s="25"/>
+      <c r="H35" s="4"/>
+      <c r="I35" s="4"/>
+      <c r="J35" s="26"/>
+    </row>
+    <row r="36" spans="1:10">
+      <c r="A36" s="3" t="s">
+        <v>561</v>
+      </c>
+      <c r="B36" s="20"/>
+      <c r="C36" s="4"/>
+      <c r="D36" s="4"/>
+      <c r="E36" s="20"/>
+      <c r="F36" s="25"/>
+      <c r="G36" s="25"/>
+      <c r="H36" s="4"/>
+      <c r="I36" s="4"/>
+      <c r="J36" s="26"/>
+    </row>
+    <row r="37" spans="1:10">
+      <c r="A37" s="3" t="s">
+        <v>561</v>
+      </c>
+      <c r="B37" s="20"/>
+      <c r="C37" s="4"/>
+      <c r="D37" s="4"/>
+      <c r="E37" s="20"/>
+      <c r="F37" s="25"/>
+      <c r="G37" s="25"/>
+      <c r="H37" s="4"/>
+      <c r="I37" s="4"/>
+      <c r="J37" s="26"/>
+    </row>
+    <row r="38" spans="1:10">
+      <c r="A38" s="3" t="s">
+        <v>561</v>
+      </c>
+      <c r="B38" s="24"/>
+      <c r="C38" s="25"/>
+      <c r="D38" s="25"/>
+      <c r="E38" s="24"/>
+      <c r="F38" s="25"/>
+      <c r="G38" s="25"/>
+      <c r="H38" s="25"/>
+      <c r="I38" s="25"/>
+      <c r="J38" s="26"/>
+    </row>
+    <row r="39" spans="1:10">
+      <c r="A39" s="5"/>
+      <c r="B39" s="6"/>
+      <c r="C39" s="6"/>
+      <c r="D39" s="6"/>
+      <c r="E39" s="6"/>
+      <c r="F39" s="6"/>
+      <c r="G39" s="6"/>
+      <c r="H39" s="6"/>
+      <c r="I39" s="6"/>
+      <c r="J39" s="8"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Atualização Controle de Tabelas Nova e Nike
</commit_message>
<xml_diff>
--- a/Documentação/Controle_Tabelas_e_Execucao/NIKE-Controle_tabelas.xlsx
+++ b/Documentação/Controle_Tabelas_e_Execucao/NIKE-Controle_tabelas.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="30" windowWidth="20115" windowHeight="8010" tabRatio="734" firstSheet="3" activeTab="9"/>
+    <workbookView xWindow="240" yWindow="30" windowWidth="20115" windowHeight="8010" tabRatio="734" firstSheet="2" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Controladores Nike" sheetId="2" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2017" uniqueCount="590">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2140" uniqueCount="642">
   <si>
     <t>dtsx Principal</t>
   </si>
@@ -1720,79 +1720,235 @@
     <t>(DFT) Nike - Cliente Varejo</t>
   </si>
   <si>
-    <t>[nike].[stg_clientes_varejo]</t>
-  </si>
-  <si>
     <t>(DFT) Nike - Estq Prod Entra Sai</t>
   </si>
   <si>
-    <t>[nike].[stg_estoque_prod_ent_sai]</t>
-  </si>
-  <si>
     <t>(DFT) Nike - Estq Prod1 Entra Sai</t>
   </si>
   <si>
-    <t>[nike].[stg_estoque_prod1_ent_sai]</t>
-  </si>
-  <si>
     <t>(DFT) Nike - Loja Entra Sai</t>
   </si>
   <si>
-    <t>[nike].[stg_loja_ent_sai]</t>
-  </si>
-  <si>
     <t>(DFT) Nike - Loja Entra Sai Produto</t>
   </si>
   <si>
-    <t>[nike].[stg_loja_ent_sai_produto]</t>
-  </si>
-  <si>
     <t>(DFT) Nike - Loja Imposto</t>
   </si>
   <si>
-    <t>[nike].[stg_loja_imposto]</t>
-  </si>
-  <si>
     <t>(DFT) Nike - Loja NF</t>
   </si>
   <si>
-    <t>[nike].[stg_loja_nf]</t>
-  </si>
-  <si>
     <t>(DFT) Nike - Loja NF Item</t>
   </si>
   <si>
-    <t>[nike].[stg_loja_nf_item]</t>
-  </si>
-  <si>
     <t>(DFT) Nike - Loja Venda</t>
   </si>
   <si>
-    <t>[nike].[stg_loja_venda]</t>
-  </si>
-  <si>
     <t>(DFT) Nike - Loja Venda Pagto</t>
   </si>
   <si>
-    <t>[nike].[stg_loja_venda_pagto]</t>
-  </si>
-  <si>
     <t>(DFT) Nike - Loja Vda Pagto Parcelas</t>
   </si>
   <si>
-    <t>[nike].[stg_loja_venda_pagto_parcelas]</t>
-  </si>
-  <si>
     <t>(DFT) Nike - Loja Vda Produto</t>
   </si>
   <si>
-    <t>[nike].[stg_loja_venda_produto]</t>
-  </si>
-  <si>
     <t>(DFT) Nike - Loja Vda Troca</t>
   </si>
   <si>
-    <t>[nike].[stg_loja_venda_troca]</t>
+    <t>N:\Migracao\Nike_Carga\Nike_Carga\stg_carga_ln_ehub.dtsx</t>
+  </si>
+  <si>
+    <t>(SC) Carrega Ehub</t>
+  </si>
+  <si>
+    <t>(DFT) Carga Clientes Varejo</t>
+  </si>
+  <si>
+    <t>(DFT) Loja Venda</t>
+  </si>
+  <si>
+    <t>(DFT) Loja NF</t>
+  </si>
+  <si>
+    <t>(DFT) Loja Entr Sai</t>
+  </si>
+  <si>
+    <t>(DFT) Loja Venda Produto</t>
+  </si>
+  <si>
+    <t>(DFT) Loja NF Item</t>
+  </si>
+  <si>
+    <t>(DFT) Loja Entr Sai Produto</t>
+  </si>
+  <si>
+    <t>(DFT) Loja Venda Pagamento</t>
+  </si>
+  <si>
+    <t>(DFT) Loja NF Imposto</t>
+  </si>
+  <si>
+    <t>(DFT) Loja Venda Troca</t>
+  </si>
+  <si>
+    <t>(DFT) Loja Venda Pagto Parcela</t>
+  </si>
+  <si>
+    <t>N:\Migracao\Nike_Carga\Nike_Carga\stg_integracao_dados_clientes.dtsx</t>
+  </si>
+  <si>
+    <t>(SC) Carga Stage</t>
+  </si>
+  <si>
+    <t>(SC) Carga ODS</t>
+  </si>
+  <si>
+    <t>N:\Migracao\Nike_Carga\Nike_Carga\stg_instancia_nike.dtsx</t>
+  </si>
+  <si>
+    <t>(SC) Carrega Informações de Instâncias</t>
+  </si>
+  <si>
+    <t>(DFT) Instâncias Troca e Estorno</t>
+  </si>
+  <si>
+    <t>(DFT) Instâncias - Clientes</t>
+  </si>
+  <si>
+    <t>(DFT) Instâncias - Endereços</t>
+  </si>
+  <si>
+    <t>N:\Migracao\Nike_Carga\Nike_Carga\ods_instancia_nike.dtsx</t>
+  </si>
+  <si>
+    <t>(SC) ODS Instancias Nike</t>
+  </si>
+  <si>
+    <t>(DFT) ODS Instâncias Encerradas</t>
+  </si>
+  <si>
+    <t>(DFT) ODS Instâncias Troca e Estorno</t>
+  </si>
+  <si>
+    <t>(DFT) ODS Instâncias Clientes</t>
+  </si>
+  <si>
+    <t>(DFT) ODS Instâncias Endereços</t>
+  </si>
+  <si>
+    <t>nike.stg_clientes_varejo</t>
+  </si>
+  <si>
+    <t>nike.stg_estoque_prod_ent_sai</t>
+  </si>
+  <si>
+    <t>nike.stg_estoque_prod1_ent_sai</t>
+  </si>
+  <si>
+    <t>nike.stg_loja_ent_sai</t>
+  </si>
+  <si>
+    <t>nike.stg_loja_ent_sai_produto</t>
+  </si>
+  <si>
+    <t>nike.stg_loja_imposto</t>
+  </si>
+  <si>
+    <t>nike.stg_loja_nf</t>
+  </si>
+  <si>
+    <t>nike.stg_loja_nf_item</t>
+  </si>
+  <si>
+    <t>nike.stg_loja_venda</t>
+  </si>
+  <si>
+    <t>nike.stg_loja_venda_pagto</t>
+  </si>
+  <si>
+    <t>nike.stg_loja_venda_pagto_parcelas</t>
+  </si>
+  <si>
+    <t>nike.stg_loja_venda_produto</t>
+  </si>
+  <si>
+    <t>nike.stg_loja_venda_troca</t>
+  </si>
+  <si>
+    <t>nk_mig.stg_clientes_varejo</t>
+  </si>
+  <si>
+    <t>nk_mig.stg_loja_venda</t>
+  </si>
+  <si>
+    <t>nk_mig.stg_loja_nf</t>
+  </si>
+  <si>
+    <t>nk_mig.stg_loja_ent_sai</t>
+  </si>
+  <si>
+    <t>nk_mig.stg_loja_venda_produto</t>
+  </si>
+  <si>
+    <t>nk_mig.stg_loja_nf_item</t>
+  </si>
+  <si>
+    <t>nk_mig.stg_loja_ent_sai_produto</t>
+  </si>
+  <si>
+    <t>nk_mig.stg_loja_venda_pgto</t>
+  </si>
+  <si>
+    <t>nk_mig.stg_loja_nf_imposto</t>
+  </si>
+  <si>
+    <t>nk_mig.stg_loja_venda_troca</t>
+  </si>
+  <si>
+    <t>nk_mig.stg_loja_venda_pgto_parcelas</t>
+  </si>
+  <si>
+    <t>nike.stg_dados_clientes</t>
+  </si>
+  <si>
+    <t>nike.ods_dados_clientes</t>
+  </si>
+  <si>
+    <t>nike.aux_dados_clientes</t>
+  </si>
+  <si>
+    <t>nike.stg_instancias_troca_estorno</t>
+  </si>
+  <si>
+    <t>nike.stg_intancia_clientes</t>
+  </si>
+  <si>
+    <t>nike.stg_instancias_endereco</t>
+  </si>
+  <si>
+    <t>nike.ods_instancias_encerradas</t>
+  </si>
+  <si>
+    <t>nike.aux_instancias_encerradas</t>
+  </si>
+  <si>
+    <t>nike.ods_instancias_troca_estorno</t>
+  </si>
+  <si>
+    <t>nike.aux_instancias_troca_estorno</t>
+  </si>
+  <si>
+    <t>nike.ods_instancia_clientes</t>
+  </si>
+  <si>
+    <t>nike.aux_instancia_clientes</t>
+  </si>
+  <si>
+    <t>nike.ods_instancias_endereco</t>
+  </si>
+  <si>
+    <t>nike.aux_instancias_endereco</t>
   </si>
 </sst>
 </file>
@@ -2892,11 +3048,11 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J39"/>
+  <dimension ref="A1:J42"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E18" sqref="E18"/>
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I1" sqref="I1:I1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12"/>
@@ -2906,7 +3062,7 @@
     <col min="3" max="3" width="31.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="22.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="61.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="32" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="33.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14.85546875" style="1" customWidth="1"/>
     <col min="9" max="9" width="40.5703125" style="1" bestFit="1" customWidth="1"/>
@@ -2966,7 +3122,7 @@
         <v>68</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>565</v>
+        <v>604</v>
       </c>
       <c r="J2" s="7"/>
     </row>
@@ -2984,13 +3140,13 @@
         <v>563</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="H3" s="4" t="s">
         <v>68</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>567</v>
+        <v>605</v>
       </c>
       <c r="J3" s="7"/>
     </row>
@@ -3008,13 +3164,13 @@
         <v>563</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="H4" s="4" t="s">
         <v>68</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>569</v>
+        <v>606</v>
       </c>
       <c r="J4" s="7"/>
     </row>
@@ -3032,13 +3188,13 @@
         <v>563</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>570</v>
+        <v>567</v>
       </c>
       <c r="H5" s="4" t="s">
         <v>68</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>571</v>
+        <v>607</v>
       </c>
       <c r="J5" s="7"/>
     </row>
@@ -3056,13 +3212,13 @@
         <v>563</v>
       </c>
       <c r="G6" s="25" t="s">
-        <v>572</v>
+        <v>568</v>
       </c>
       <c r="H6" s="4" t="s">
         <v>68</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>573</v>
+        <v>608</v>
       </c>
       <c r="J6" s="26"/>
     </row>
@@ -3080,13 +3236,13 @@
         <v>563</v>
       </c>
       <c r="G7" s="25" t="s">
-        <v>574</v>
+        <v>569</v>
       </c>
       <c r="H7" s="4" t="s">
         <v>68</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>575</v>
+        <v>609</v>
       </c>
       <c r="J7" s="26"/>
     </row>
@@ -3104,13 +3260,13 @@
         <v>563</v>
       </c>
       <c r="G8" s="25" t="s">
-        <v>576</v>
+        <v>570</v>
       </c>
       <c r="H8" s="4" t="s">
         <v>68</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>577</v>
+        <v>610</v>
       </c>
       <c r="J8" s="26"/>
     </row>
@@ -3128,13 +3284,13 @@
         <v>563</v>
       </c>
       <c r="G9" s="25" t="s">
-        <v>578</v>
+        <v>571</v>
       </c>
       <c r="H9" s="4" t="s">
         <v>68</v>
       </c>
       <c r="I9" s="4" t="s">
-        <v>579</v>
+        <v>611</v>
       </c>
       <c r="J9" s="26"/>
     </row>
@@ -3152,13 +3308,13 @@
         <v>563</v>
       </c>
       <c r="G10" s="25" t="s">
-        <v>580</v>
+        <v>572</v>
       </c>
       <c r="H10" s="4" t="s">
         <v>68</v>
       </c>
       <c r="I10" s="4" t="s">
-        <v>581</v>
+        <v>612</v>
       </c>
       <c r="J10" s="26"/>
     </row>
@@ -3176,13 +3332,13 @@
         <v>563</v>
       </c>
       <c r="G11" s="25" t="s">
-        <v>582</v>
+        <v>573</v>
       </c>
       <c r="H11" s="4" t="s">
         <v>68</v>
       </c>
       <c r="I11" s="4" t="s">
-        <v>583</v>
+        <v>613</v>
       </c>
       <c r="J11" s="26"/>
     </row>
@@ -3200,13 +3356,13 @@
         <v>563</v>
       </c>
       <c r="G12" s="25" t="s">
-        <v>584</v>
+        <v>574</v>
       </c>
       <c r="H12" s="4" t="s">
         <v>68</v>
       </c>
       <c r="I12" s="4" t="s">
-        <v>585</v>
+        <v>614</v>
       </c>
       <c r="J12" s="26"/>
     </row>
@@ -3224,13 +3380,13 @@
         <v>563</v>
       </c>
       <c r="G13" s="25" t="s">
-        <v>586</v>
+        <v>575</v>
       </c>
       <c r="H13" s="4" t="s">
         <v>68</v>
       </c>
       <c r="I13" s="4" t="s">
-        <v>587</v>
+        <v>615</v>
       </c>
       <c r="J13" s="26"/>
     </row>
@@ -3248,13 +3404,13 @@
         <v>563</v>
       </c>
       <c r="G14" s="25" t="s">
-        <v>588</v>
+        <v>576</v>
       </c>
       <c r="H14" s="4" t="s">
         <v>68</v>
       </c>
       <c r="I14" s="4" t="s">
-        <v>589</v>
+        <v>616</v>
       </c>
       <c r="J14" s="26"/>
     </row>
@@ -3265,11 +3421,21 @@
       <c r="B15" s="20"/>
       <c r="C15" s="4"/>
       <c r="D15" s="4"/>
-      <c r="E15" s="20"/>
-      <c r="F15" s="25"/>
-      <c r="G15" s="25"/>
-      <c r="H15" s="4"/>
-      <c r="I15" s="4"/>
+      <c r="E15" s="20" t="s">
+        <v>577</v>
+      </c>
+      <c r="F15" s="25" t="s">
+        <v>578</v>
+      </c>
+      <c r="G15" s="25" t="s">
+        <v>579</v>
+      </c>
+      <c r="H15" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="I15" s="4" t="s">
+        <v>617</v>
+      </c>
       <c r="J15" s="26"/>
     </row>
     <row r="16" spans="1:10">
@@ -3279,11 +3445,21 @@
       <c r="B16" s="20"/>
       <c r="C16" s="4"/>
       <c r="D16" s="4"/>
-      <c r="E16" s="20"/>
-      <c r="F16" s="25"/>
-      <c r="G16" s="25"/>
-      <c r="H16" s="4"/>
-      <c r="I16" s="4"/>
+      <c r="E16" s="20" t="s">
+        <v>577</v>
+      </c>
+      <c r="F16" s="25" t="s">
+        <v>578</v>
+      </c>
+      <c r="G16" s="25" t="s">
+        <v>580</v>
+      </c>
+      <c r="H16" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="I16" s="4" t="s">
+        <v>618</v>
+      </c>
       <c r="J16" s="26"/>
     </row>
     <row r="17" spans="1:10">
@@ -3293,11 +3469,21 @@
       <c r="B17" s="20"/>
       <c r="C17" s="4"/>
       <c r="D17" s="4"/>
-      <c r="E17" s="20"/>
-      <c r="F17" s="25"/>
-      <c r="G17" s="25"/>
-      <c r="H17" s="4"/>
-      <c r="I17" s="4"/>
+      <c r="E17" s="20" t="s">
+        <v>577</v>
+      </c>
+      <c r="F17" s="25" t="s">
+        <v>578</v>
+      </c>
+      <c r="G17" s="25" t="s">
+        <v>581</v>
+      </c>
+      <c r="H17" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="I17" s="4" t="s">
+        <v>619</v>
+      </c>
       <c r="J17" s="26"/>
     </row>
     <row r="18" spans="1:10">
@@ -3307,11 +3493,21 @@
       <c r="B18" s="20"/>
       <c r="C18" s="4"/>
       <c r="D18" s="4"/>
-      <c r="E18" s="20"/>
-      <c r="F18" s="25"/>
-      <c r="G18" s="25"/>
-      <c r="H18" s="4"/>
-      <c r="I18" s="4"/>
+      <c r="E18" s="20" t="s">
+        <v>577</v>
+      </c>
+      <c r="F18" s="25" t="s">
+        <v>578</v>
+      </c>
+      <c r="G18" s="25" t="s">
+        <v>582</v>
+      </c>
+      <c r="H18" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="I18" s="4" t="s">
+        <v>620</v>
+      </c>
       <c r="J18" s="26"/>
     </row>
     <row r="19" spans="1:10">
@@ -3321,11 +3517,21 @@
       <c r="B19" s="20"/>
       <c r="C19" s="4"/>
       <c r="D19" s="4"/>
-      <c r="E19" s="20"/>
-      <c r="F19" s="25"/>
-      <c r="G19" s="25"/>
-      <c r="H19" s="4"/>
-      <c r="I19" s="4"/>
+      <c r="E19" s="20" t="s">
+        <v>577</v>
+      </c>
+      <c r="F19" s="25" t="s">
+        <v>578</v>
+      </c>
+      <c r="G19" s="25" t="s">
+        <v>583</v>
+      </c>
+      <c r="H19" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="I19" s="4" t="s">
+        <v>621</v>
+      </c>
       <c r="J19" s="26"/>
     </row>
     <row r="20" spans="1:10">
@@ -3335,11 +3541,21 @@
       <c r="B20" s="20"/>
       <c r="C20" s="4"/>
       <c r="D20" s="4"/>
-      <c r="E20" s="20"/>
-      <c r="F20" s="25"/>
-      <c r="G20" s="25"/>
-      <c r="H20" s="4"/>
-      <c r="I20" s="4"/>
+      <c r="E20" s="20" t="s">
+        <v>577</v>
+      </c>
+      <c r="F20" s="25" t="s">
+        <v>578</v>
+      </c>
+      <c r="G20" s="25" t="s">
+        <v>584</v>
+      </c>
+      <c r="H20" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="I20" s="4" t="s">
+        <v>622</v>
+      </c>
       <c r="J20" s="26"/>
     </row>
     <row r="21" spans="1:10">
@@ -3349,11 +3565,21 @@
       <c r="B21" s="20"/>
       <c r="C21" s="4"/>
       <c r="D21" s="4"/>
-      <c r="E21" s="20"/>
-      <c r="F21" s="25"/>
-      <c r="G21" s="25"/>
-      <c r="H21" s="4"/>
-      <c r="I21" s="4"/>
+      <c r="E21" s="20" t="s">
+        <v>577</v>
+      </c>
+      <c r="F21" s="25" t="s">
+        <v>578</v>
+      </c>
+      <c r="G21" s="25" t="s">
+        <v>585</v>
+      </c>
+      <c r="H21" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="I21" s="4" t="s">
+        <v>623</v>
+      </c>
       <c r="J21" s="26"/>
     </row>
     <row r="22" spans="1:10">
@@ -3363,11 +3589,21 @@
       <c r="B22" s="20"/>
       <c r="C22" s="4"/>
       <c r="D22" s="4"/>
-      <c r="E22" s="20"/>
-      <c r="F22" s="25"/>
-      <c r="G22" s="25"/>
-      <c r="H22" s="4"/>
-      <c r="I22" s="4"/>
+      <c r="E22" s="20" t="s">
+        <v>577</v>
+      </c>
+      <c r="F22" s="25" t="s">
+        <v>578</v>
+      </c>
+      <c r="G22" s="25" t="s">
+        <v>586</v>
+      </c>
+      <c r="H22" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="I22" s="4" t="s">
+        <v>624</v>
+      </c>
       <c r="J22" s="26"/>
     </row>
     <row r="23" spans="1:10">
@@ -3377,11 +3613,21 @@
       <c r="B23" s="20"/>
       <c r="C23" s="4"/>
       <c r="D23" s="4"/>
-      <c r="E23" s="20"/>
-      <c r="F23" s="25"/>
-      <c r="G23" s="25"/>
-      <c r="H23" s="4"/>
-      <c r="I23" s="4"/>
+      <c r="E23" s="20" t="s">
+        <v>577</v>
+      </c>
+      <c r="F23" s="25" t="s">
+        <v>578</v>
+      </c>
+      <c r="G23" s="25" t="s">
+        <v>587</v>
+      </c>
+      <c r="H23" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="I23" s="4" t="s">
+        <v>625</v>
+      </c>
       <c r="J23" s="26"/>
     </row>
     <row r="24" spans="1:10">
@@ -3391,11 +3637,21 @@
       <c r="B24" s="20"/>
       <c r="C24" s="4"/>
       <c r="D24" s="4"/>
-      <c r="E24" s="20"/>
-      <c r="F24" s="25"/>
-      <c r="G24" s="25"/>
-      <c r="H24" s="4"/>
-      <c r="I24" s="4"/>
+      <c r="E24" s="20" t="s">
+        <v>577</v>
+      </c>
+      <c r="F24" s="25" t="s">
+        <v>578</v>
+      </c>
+      <c r="G24" s="25" t="s">
+        <v>588</v>
+      </c>
+      <c r="H24" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="I24" s="4" t="s">
+        <v>626</v>
+      </c>
       <c r="J24" s="26"/>
     </row>
     <row r="25" spans="1:10">
@@ -3405,11 +3661,21 @@
       <c r="B25" s="20"/>
       <c r="C25" s="4"/>
       <c r="D25" s="4"/>
-      <c r="E25" s="20"/>
-      <c r="F25" s="25"/>
-      <c r="G25" s="25"/>
-      <c r="H25" s="4"/>
-      <c r="I25" s="4"/>
+      <c r="E25" s="20" t="s">
+        <v>577</v>
+      </c>
+      <c r="F25" s="25" t="s">
+        <v>578</v>
+      </c>
+      <c r="G25" s="25" t="s">
+        <v>589</v>
+      </c>
+      <c r="H25" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="I25" s="4" t="s">
+        <v>627</v>
+      </c>
       <c r="J25" s="26"/>
     </row>
     <row r="26" spans="1:10">
@@ -3419,11 +3685,21 @@
       <c r="B26" s="20"/>
       <c r="C26" s="4"/>
       <c r="D26" s="4"/>
-      <c r="E26" s="20"/>
-      <c r="F26" s="25"/>
-      <c r="G26" s="25"/>
-      <c r="H26" s="4"/>
-      <c r="I26" s="4"/>
+      <c r="E26" s="20" t="s">
+        <v>590</v>
+      </c>
+      <c r="F26" s="25" t="s">
+        <v>591</v>
+      </c>
+      <c r="G26" s="25" t="s">
+        <v>289</v>
+      </c>
+      <c r="H26" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="I26" s="4" t="s">
+        <v>628</v>
+      </c>
       <c r="J26" s="26"/>
     </row>
     <row r="27" spans="1:10">
@@ -3433,11 +3709,21 @@
       <c r="B27" s="20"/>
       <c r="C27" s="4"/>
       <c r="D27" s="4"/>
-      <c r="E27" s="20"/>
-      <c r="F27" s="25"/>
-      <c r="G27" s="25"/>
-      <c r="H27" s="4"/>
-      <c r="I27" s="4"/>
+      <c r="E27" s="20" t="s">
+        <v>590</v>
+      </c>
+      <c r="F27" s="25" t="s">
+        <v>592</v>
+      </c>
+      <c r="G27" s="25" t="s">
+        <v>291</v>
+      </c>
+      <c r="H27" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="I27" s="4" t="s">
+        <v>629</v>
+      </c>
       <c r="J27" s="26"/>
     </row>
     <row r="28" spans="1:10">
@@ -3447,11 +3733,21 @@
       <c r="B28" s="20"/>
       <c r="C28" s="4"/>
       <c r="D28" s="4"/>
-      <c r="E28" s="20"/>
-      <c r="F28" s="25"/>
-      <c r="G28" s="25"/>
-      <c r="H28" s="4"/>
-      <c r="I28" s="4"/>
+      <c r="E28" s="20" t="s">
+        <v>590</v>
+      </c>
+      <c r="F28" s="25" t="s">
+        <v>592</v>
+      </c>
+      <c r="G28" s="25" t="s">
+        <v>291</v>
+      </c>
+      <c r="H28" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="I28" s="4" t="s">
+        <v>630</v>
+      </c>
       <c r="J28" s="26"/>
     </row>
     <row r="29" spans="1:10">
@@ -3461,11 +3757,21 @@
       <c r="B29" s="20"/>
       <c r="C29" s="4"/>
       <c r="D29" s="4"/>
-      <c r="E29" s="20"/>
-      <c r="F29" s="25"/>
-      <c r="G29" s="25"/>
-      <c r="H29" s="4"/>
-      <c r="I29" s="4"/>
+      <c r="E29" s="20" t="s">
+        <v>593</v>
+      </c>
+      <c r="F29" s="25" t="s">
+        <v>594</v>
+      </c>
+      <c r="G29" s="25" t="s">
+        <v>595</v>
+      </c>
+      <c r="H29" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="I29" s="4" t="s">
+        <v>631</v>
+      </c>
       <c r="J29" s="26"/>
     </row>
     <row r="30" spans="1:10">
@@ -3475,11 +3781,21 @@
       <c r="B30" s="20"/>
       <c r="C30" s="4"/>
       <c r="D30" s="4"/>
-      <c r="E30" s="20"/>
-      <c r="F30" s="25"/>
-      <c r="G30" s="25"/>
-      <c r="H30" s="4"/>
-      <c r="I30" s="4"/>
+      <c r="E30" s="20" t="s">
+        <v>593</v>
+      </c>
+      <c r="F30" s="25" t="s">
+        <v>594</v>
+      </c>
+      <c r="G30" s="25" t="s">
+        <v>596</v>
+      </c>
+      <c r="H30" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="I30" s="4" t="s">
+        <v>632</v>
+      </c>
       <c r="J30" s="26"/>
     </row>
     <row r="31" spans="1:10">
@@ -3489,13 +3805,21 @@
       <c r="B31" s="20"/>
       <c r="C31" s="4"/>
       <c r="D31" s="4"/>
-      <c r="E31" s="20"/>
-      <c r="F31" s="25"/>
-      <c r="G31" s="25"/>
+      <c r="E31" s="20" t="s">
+        <v>593</v>
+      </c>
+      <c r="F31" s="25" t="s">
+        <v>594</v>
+      </c>
+      <c r="G31" s="25" t="s">
+        <v>597</v>
+      </c>
       <c r="H31" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="I31" s="4"/>
+        <v>161</v>
+      </c>
+      <c r="I31" s="4" t="s">
+        <v>633</v>
+      </c>
       <c r="J31" s="26"/>
     </row>
     <row r="32" spans="1:10">
@@ -3505,13 +3829,21 @@
       <c r="B32" s="20"/>
       <c r="C32" s="4"/>
       <c r="D32" s="4"/>
-      <c r="E32" s="20"/>
-      <c r="F32" s="25"/>
-      <c r="G32" s="25"/>
+      <c r="E32" s="20" t="s">
+        <v>598</v>
+      </c>
+      <c r="F32" s="25" t="s">
+        <v>599</v>
+      </c>
+      <c r="G32" s="25" t="s">
+        <v>600</v>
+      </c>
       <c r="H32" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="I32" s="4"/>
+        <v>161</v>
+      </c>
+      <c r="I32" s="4" t="s">
+        <v>634</v>
+      </c>
       <c r="J32" s="26"/>
     </row>
     <row r="33" spans="1:10">
@@ -3521,13 +3853,21 @@
       <c r="B33" s="20"/>
       <c r="C33" s="4"/>
       <c r="D33" s="4"/>
-      <c r="E33" s="20"/>
-      <c r="F33" s="25"/>
-      <c r="G33" s="25"/>
+      <c r="E33" s="20" t="s">
+        <v>598</v>
+      </c>
+      <c r="F33" s="25" t="s">
+        <v>599</v>
+      </c>
+      <c r="G33" s="25" t="s">
+        <v>600</v>
+      </c>
       <c r="H33" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="I33" s="4"/>
+        <v>161</v>
+      </c>
+      <c r="I33" s="4" t="s">
+        <v>635</v>
+      </c>
       <c r="J33" s="26"/>
     </row>
     <row r="34" spans="1:10">
@@ -3537,11 +3877,21 @@
       <c r="B34" s="20"/>
       <c r="C34" s="4"/>
       <c r="D34" s="4"/>
-      <c r="E34" s="20"/>
-      <c r="F34" s="25"/>
-      <c r="G34" s="25"/>
-      <c r="H34" s="4"/>
-      <c r="I34" s="4"/>
+      <c r="E34" s="20" t="s">
+        <v>598</v>
+      </c>
+      <c r="F34" s="25" t="s">
+        <v>599</v>
+      </c>
+      <c r="G34" s="25" t="s">
+        <v>601</v>
+      </c>
+      <c r="H34" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="I34" s="4" t="s">
+        <v>636</v>
+      </c>
       <c r="J34" s="26"/>
     </row>
     <row r="35" spans="1:10">
@@ -3551,11 +3901,21 @@
       <c r="B35" s="20"/>
       <c r="C35" s="4"/>
       <c r="D35" s="4"/>
-      <c r="E35" s="20"/>
-      <c r="F35" s="25"/>
-      <c r="G35" s="25"/>
-      <c r="H35" s="4"/>
-      <c r="I35" s="4"/>
+      <c r="E35" s="20" t="s">
+        <v>598</v>
+      </c>
+      <c r="F35" s="25" t="s">
+        <v>599</v>
+      </c>
+      <c r="G35" s="25" t="s">
+        <v>601</v>
+      </c>
+      <c r="H35" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="I35" s="4" t="s">
+        <v>637</v>
+      </c>
       <c r="J35" s="26"/>
     </row>
     <row r="36" spans="1:10">
@@ -3565,11 +3925,21 @@
       <c r="B36" s="20"/>
       <c r="C36" s="4"/>
       <c r="D36" s="4"/>
-      <c r="E36" s="20"/>
-      <c r="F36" s="25"/>
-      <c r="G36" s="25"/>
-      <c r="H36" s="4"/>
-      <c r="I36" s="4"/>
+      <c r="E36" s="20" t="s">
+        <v>598</v>
+      </c>
+      <c r="F36" s="25" t="s">
+        <v>599</v>
+      </c>
+      <c r="G36" s="25" t="s">
+        <v>602</v>
+      </c>
+      <c r="H36" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="I36" s="4" t="s">
+        <v>638</v>
+      </c>
       <c r="J36" s="26"/>
     </row>
     <row r="37" spans="1:10">
@@ -3579,38 +3949,106 @@
       <c r="B37" s="20"/>
       <c r="C37" s="4"/>
       <c r="D37" s="4"/>
-      <c r="E37" s="20"/>
-      <c r="F37" s="25"/>
-      <c r="G37" s="25"/>
-      <c r="H37" s="4"/>
-      <c r="I37" s="4"/>
+      <c r="E37" s="20" t="s">
+        <v>598</v>
+      </c>
+      <c r="F37" s="25" t="s">
+        <v>599</v>
+      </c>
+      <c r="G37" s="25" t="s">
+        <v>602</v>
+      </c>
+      <c r="H37" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="I37" s="4" t="s">
+        <v>639</v>
+      </c>
       <c r="J37" s="26"/>
     </row>
     <row r="38" spans="1:10">
       <c r="A38" s="3" t="s">
         <v>561</v>
       </c>
-      <c r="B38" s="24"/>
-      <c r="C38" s="25"/>
-      <c r="D38" s="25"/>
-      <c r="E38" s="24"/>
-      <c r="F38" s="25"/>
-      <c r="G38" s="25"/>
-      <c r="H38" s="25"/>
-      <c r="I38" s="25"/>
+      <c r="B38" s="20"/>
+      <c r="C38" s="4"/>
+      <c r="D38" s="4"/>
+      <c r="E38" s="20" t="s">
+        <v>598</v>
+      </c>
+      <c r="F38" s="25" t="s">
+        <v>599</v>
+      </c>
+      <c r="G38" s="25" t="s">
+        <v>603</v>
+      </c>
+      <c r="H38" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="I38" s="4" t="s">
+        <v>640</v>
+      </c>
       <c r="J38" s="26"/>
     </row>
     <row r="39" spans="1:10">
-      <c r="A39" s="5"/>
-      <c r="B39" s="6"/>
-      <c r="C39" s="6"/>
-      <c r="D39" s="6"/>
-      <c r="E39" s="6"/>
-      <c r="F39" s="6"/>
-      <c r="G39" s="6"/>
-      <c r="H39" s="6"/>
-      <c r="I39" s="6"/>
-      <c r="J39" s="8"/>
+      <c r="A39" s="3" t="s">
+        <v>561</v>
+      </c>
+      <c r="B39" s="20"/>
+      <c r="C39" s="4"/>
+      <c r="D39" s="4"/>
+      <c r="E39" s="20" t="s">
+        <v>598</v>
+      </c>
+      <c r="F39" s="25" t="s">
+        <v>599</v>
+      </c>
+      <c r="G39" s="25" t="s">
+        <v>603</v>
+      </c>
+      <c r="H39" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="I39" s="4" t="s">
+        <v>641</v>
+      </c>
+      <c r="J39" s="26"/>
+    </row>
+    <row r="40" spans="1:10">
+      <c r="A40" s="3"/>
+      <c r="B40" s="20"/>
+      <c r="C40" s="4"/>
+      <c r="D40" s="4"/>
+      <c r="E40" s="20"/>
+      <c r="F40" s="25"/>
+      <c r="G40" s="25"/>
+      <c r="H40" s="4"/>
+      <c r="I40" s="4"/>
+      <c r="J40" s="26"/>
+    </row>
+    <row r="41" spans="1:10">
+      <c r="A41" s="3"/>
+      <c r="B41" s="24"/>
+      <c r="C41" s="25"/>
+      <c r="D41" s="25"/>
+      <c r="E41" s="24"/>
+      <c r="F41" s="25"/>
+      <c r="G41" s="25"/>
+      <c r="H41" s="4"/>
+      <c r="I41" s="25"/>
+      <c r="J41" s="26"/>
+    </row>
+    <row r="42" spans="1:10">
+      <c r="A42" s="5"/>
+      <c r="B42" s="6"/>
+      <c r="C42" s="6"/>
+      <c r="D42" s="6"/>
+      <c r="E42" s="6"/>
+      <c r="F42" s="6"/>
+      <c r="G42" s="6"/>
+      <c r="H42" s="6"/>
+      <c r="I42" s="6"/>
+      <c r="J42" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -9374,9 +9812,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12"/>

</xml_diff>